<commit_message>
termine el hasta el 2c
</commit_message>
<xml_diff>
--- a/TP2/2.Datos/2.c.xlsx
+++ b/TP2/2.Datos/2.c.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OperaDownload\Laboratorio Electronica\lab-electronica\.git\TP2\2.Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OperaDownload\Laboratorio Electronica\lab-electronica\TP2\2.Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87529182-D09D-438E-B167-AFEF0989FBF6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B93383-536D-4B69-8317-4E74EBA40394}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" xr2:uid="{5A9014B8-39DC-406C-892A-5EE7C928D4E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179021" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -393,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F264DA-CF6F-40B8-94A4-F2C58C55B57C}">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,7 +459,7 @@
         <v>-6</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E68" si="0">20*LOG10(C3/B3)</f>
+        <f t="shared" ref="E3:E39" si="0">20*LOG10(C3/B3)</f>
         <v>6.1576582148553305</v>
       </c>
     </row>
@@ -991,7 +996,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="D33" s="1">
-        <v>180</v>
+        <v>-180</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
@@ -1009,7 +1014,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="D34" s="1">
-        <v>173</v>
+        <v>-173</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
@@ -1027,7 +1032,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="D35" s="1">
-        <v>171</v>
+        <v>-171</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" si="0"/>
@@ -1045,7 +1050,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="D36" s="1">
-        <v>175</v>
+        <v>-175</v>
       </c>
       <c r="E36" s="1">
         <f t="shared" si="0"/>
@@ -1063,7 +1068,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="D37" s="1">
-        <v>184</v>
+        <v>-184</v>
       </c>
       <c r="E37" s="1">
         <f t="shared" si="0"/>
@@ -1081,7 +1086,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="D38" s="1">
-        <v>181</v>
+        <v>-181</v>
       </c>
       <c r="E38" s="1">
         <f t="shared" si="0"/>
@@ -1098,327 +1103,12 @@
       <c r="C39" s="1">
         <v>3.1E-2</v>
       </c>
+      <c r="D39" s="1">
+        <v>-182</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="0"/>
         <v>-30.2591935989674</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E40" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E41" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E42" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E43" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E44" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E45" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E46" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E47" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E48" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E49" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E50" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E51" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E52" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E53" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E54" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E55" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E56" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E57" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E58" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E59" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E60" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E61" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E62" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E63" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E64" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E65" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E66" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E67" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E68" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E69" s="1" t="e">
-        <f t="shared" ref="E69:E92" si="1">20*LOG10(C69/B69)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E70" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E71" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E72" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E73" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E74" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E75" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E76" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E77" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E78" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E79" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E80" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E81" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E82" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E83" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E84" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E85" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E86" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E87" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E88" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E89" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E90" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E91" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E92" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>